<commit_message>
Improved the database script and developed the user creation route
</commit_message>
<xml_diff>
--- a/DOCS/API Route Design.xlsx
+++ b/DOCS/API Route Design.xlsx
@@ -65,9 +65,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>Email, Name, Password</t>
-  </si>
-  <si>
     <t>Loging in</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>/api/collections/shared/item/:id</t>
+  </si>
+  <si>
+    <t>Name, Email, Password</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -607,243 +607,243 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Marked sign in route as done
</commit_message>
<xml_diff>
--- a/DOCS/API Route Design.xlsx
+++ b/DOCS/API Route Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>ENTITIES</t>
   </si>
@@ -174,13 +174,16 @@
   </si>
   <si>
     <t>Name, Email, Password</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +202,13 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -225,11 +235,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,7 +563,7 @@
   <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -611,6 +624,9 @@
       </c>
       <c r="H5" t="s">
         <v>49</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Developed 4 new routes on the backend, improved database script
routes developed:
-login
-viewing a user's collections
-adding a new collection
-viewing a collection's detail

-Improved the database script, changed longblob types to blob

-Marked developed routes as DONE in the excell sheet
</commit_message>
<xml_diff>
--- a/DOCS/API Route Design.xlsx
+++ b/DOCS/API Route Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>ENTITIES</t>
   </si>
@@ -563,7 +563,7 @@
   <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -648,8 +648,11 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>19</v>
       </c>
@@ -668,8 +671,11 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>46</v>
       </c>
@@ -688,8 +694,11 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
         <v>23</v>
       </c>
@@ -707,6 +716,9 @@
       </c>
       <c r="H9" t="s">
         <v>25</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Marked newly developed routes as DONE
Marked Routes:
-Add an item to a collection
-Edit an item's info
-Delete an item
-Unlist a collection
-Relist a collection
</commit_message>
<xml_diff>
--- a/DOCS/API Route Design.xlsx
+++ b/DOCS/API Route Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>ENTITIES</t>
   </si>
@@ -563,7 +563,7 @@
   <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
         <v>26</v>
       </c>
@@ -740,8 +740,11 @@
       <c r="H10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -760,8 +763,11 @@
       <c r="H11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>33</v>
       </c>
@@ -780,8 +786,11 @@
       <c r="H12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -800,8 +809,11 @@
       <c r="H13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>39</v>
       </c>
@@ -819,6 +831,9 @@
       </c>
       <c r="H14" t="s">
         <v>18</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>